<commit_message>
Aggiornato file base.xlsx adattandolo a nuovi dati nella misurazione
</commit_message>
<xml_diff>
--- a/ProgettoFormLetturaDati/examples/base.xlsx
+++ b/ProgettoFormLetturaDati/examples/base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\ProgettoOMB\ProgettoFormLetturaDati\HydrogenOMB\bin\Debug\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8AC135-BFF8-4BE4-8D4E-C7D7998856A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26AFCC-466E-4BE7-98EC-E2F033BACFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatiGenerali" sheetId="4" r:id="rId1"/>
@@ -19,13 +19,12 @@
     <sheet name="Grafico" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="AngoloApertura">OFFSET(MisurazioniApertura!$C$2,0,0,MisurazioniApertura!$F$1)</definedName>
-    <definedName name="AngoloChiusura">OFFSET(MisurazioniChiusura!$C$2,0,0,MisurazioniChiusura!$F$1)</definedName>
-    <definedName name="TrimmerApertura">OFFSET(MisurazioniApertura!$D$2,0,0,MisurazioniApertura!$F$1)</definedName>
-    <definedName name="TrimmerChiusura">OFFSET(MisurazioniChiusura!$D$2,0,0,MisurazioniChiusura!$F$1)</definedName>
+    <definedName name="AngoloApertura">OFFSET(MisurazioniApertura!$A$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="AngoloChiusura">OFFSET(MisurazioniChiusura!$A$2,0,0,MisurazioniChiusura!$F$1)</definedName>
+    <definedName name="TrimmerApertura">OFFSET(MisurazioniApertura!$B$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="TrimmerChiusura">OFFSET(MisurazioniChiusura!$B$2,0,0,MisurazioniChiusura!$F$1)</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -231,7 +230,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -239,7 +238,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -544,7 +543,7 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:numRef>
+                  <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -552,7 +551,7 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:numRef>
+                  </c:multiLvlStrRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -2162,20 +2161,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2189,21 +2188,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669F6F74-513D-4C94-B6DE-E93AC5E8854B}">
   <dimension ref="C1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
       <c r="F1" s="1">
-        <f>COUNT(C:C)</f>
+        <f>COUNT(A:A)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C2" s="2"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="F5" s="2"/>
     </row>
   </sheetData>
@@ -2216,13 +2217,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E58275-41A7-4F03-A451-BBB72D77F0A2}">
   <dimension ref="F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F1" s="1">
-        <f>COUNT(C:C)</f>
+        <f>COUNT(A:A)</f>
         <v>0</v>
       </c>
     </row>
@@ -2235,11 +2238,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26ADF7C-3EEE-44EB-BC6C-C3F011005C33}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file base.xlsx per rispettare nuovi parametri accettati
</commit_message>
<xml_diff>
--- a/ProgettoFormLetturaDati/examples/base.xlsx
+++ b/ProgettoFormLetturaDati/examples/base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principale\source\repos\ProgettoOMB\ProgettoFormLetturaDati\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26AFCC-466E-4BE7-98EC-E2F033BACFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A92807-E39B-45F7-9915-483D6D0A911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-300" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatiGenerali" sheetId="4" r:id="rId1"/>
@@ -24,22 +24,30 @@
     <definedName name="TrimmerApertura">OFFSET(MisurazioniApertura!$B$2,0,0,MisurazioniApertura!$F$1)</definedName>
     <definedName name="TrimmerChiusura">OFFSET(MisurazioniChiusura!$B$2,0,0,MisurazioniChiusura!$F$1)</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>MODELLO</t>
+    <t>SERIAL NUMBER:</t>
   </si>
 </sst>
 </file>
@@ -2158,25 +2166,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF3B858-B44E-4ACE-8F25-54A412D81C95}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2192,19 +2195,19 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F1" s="1">
         <f>COUNT(A:A)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F5" s="2"/>
     </row>
   </sheetData>
@@ -2221,9 +2224,9 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1" s="1">
         <f>COUNT(A:A)</f>
         <v>0</v>
@@ -2238,13 +2241,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26ADF7C-3EEE-44EB-BC6C-C3F011005C33}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
   </sheetData>

</xml_diff>